<commit_message>
new code variants for different purposes
I am working on a presentation and therefore collect my Data and update figures + graphs.
</commit_message>
<xml_diff>
--- a/data_tables/GSH_depletion.xlsx
+++ b/data_tables/GSH_depletion.xlsx
@@ -1,54 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miri\OneDrive\Desktop\R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rickman\Documents\GitHub\R-graphs\data_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21DF3D0F-ACF3-48FB-841F-33E3ADFD6932}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7806F054-D8DC-468F-A840-9939D35AC14B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="2" xr2:uid="{5A086EDC-5365-44F2-90FD-DF3D8A971B89}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5A086EDC-5365-44F2-90FD-DF3D8A971B89}"/>
   </bookViews>
   <sheets>
     <sheet name="alldata" sheetId="1" r:id="rId1"/>
     <sheet name="table" sheetId="3" r:id="rId2"/>
     <sheet name="SEM" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="14">
   <si>
     <t>S1</t>
   </si>
   <si>
-    <t>Blank</t>
-  </si>
-  <si>
-    <t>DMSO</t>
-  </si>
-  <si>
     <t>S2</t>
   </si>
   <si>
@@ -61,12 +44,6 @@
     <t>healthy</t>
   </si>
   <si>
-    <t>S5</t>
-  </si>
-  <si>
-    <t>G6PD</t>
-  </si>
-  <si>
     <t>incubation</t>
   </si>
   <si>
@@ -92,9 +69,6 @@
   </si>
   <si>
     <t>S7</t>
-  </si>
-  <si>
-    <t>S8</t>
   </si>
 </sst>
 </file>
@@ -460,220 +434,191 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76D6FC8A-E6A9-4D4E-AABC-18E337C9E6D3}">
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S13" sqref="S13:S15"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="D1">
+        <v>0.1</v>
       </c>
       <c r="E1">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="F1">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="G1">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="H1">
         <v>2</v>
       </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>2</v>
-      </c>
-      <c r="O1">
-        <v>0.1</v>
-      </c>
-      <c r="P1">
-        <v>0.25</v>
-      </c>
-      <c r="Q1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2">
-        <v>6.5569643859999998</v>
+        <v>4.0548086852306326</v>
       </c>
       <c r="D2">
-        <v>5.8973880870000004</v>
+        <v>2.9102354412683633</v>
       </c>
       <c r="E2">
-        <v>5.0865967090000002</v>
+        <v>1.376221387124291</v>
       </c>
       <c r="F2">
-        <v>2.790515112</v>
+        <v>0.92538519563920074</v>
       </c>
       <c r="G2">
-        <v>1.283338501</v>
-      </c>
-      <c r="K2" t="s">
-        <v>7</v>
-      </c>
-      <c r="L2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M2">
-        <v>1.1670344370000001</v>
-      </c>
-      <c r="N2">
-        <v>1.168250097</v>
-      </c>
-      <c r="Q2">
-        <v>0.198152722</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+        <v>0.51260660473402087</v>
+      </c>
+      <c r="H2">
+        <v>0.28267597652985732</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>4.2299977048042869</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2.9121306999439582</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1.4827084278250822</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.82720413143920724</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.39161095384085171</v>
+      </c>
+      <c r="H3">
+        <v>0.21757186427196445</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3.2189913048053285</v>
+      </c>
+      <c r="D4">
+        <v>1.6971390018855563</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.61578305768136732</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.36805424137277126</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.22256271433438937</v>
+      </c>
+      <c r="H4">
+        <v>0.16461934995840388</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1">
-        <v>6.6430248609999998</v>
-      </c>
-      <c r="D3" s="1">
-        <v>6.9331400480000003</v>
-      </c>
-      <c r="E3" s="1">
-        <v>5.4662195960000002</v>
-      </c>
-      <c r="F3" s="1">
-        <v>4.0697848749999999</v>
-      </c>
-      <c r="G3" s="1">
-        <v>2.9042164659999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1">
-        <v>5.0545252539999996</v>
-      </c>
-      <c r="D4">
-        <v>7.510890303</v>
-      </c>
-      <c r="E4" s="1">
-        <v>3.3039098729999998</v>
-      </c>
-      <c r="F4" s="1">
-        <v>2.1151244139999998</v>
-      </c>
-      <c r="G4" s="1">
-        <v>1.107135435</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C5">
-        <v>9.5332073439999991</v>
+        <v>6.3549930141391329</v>
+      </c>
+      <c r="D5">
+        <v>4.8536046049568755</v>
       </c>
       <c r="E5">
-        <v>6.7014821739999997</v>
+        <v>2.8791834201062914</v>
       </c>
       <c r="F5">
-        <v>5.5222651760000003</v>
+        <v>2.4163154500314294</v>
       </c>
       <c r="G5">
-        <v>3.1477874130000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+        <v>1.4797310418330756</v>
+      </c>
+      <c r="H5">
+        <v>0.63820992506355934</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1">
-        <v>5.4943207049999998</v>
+        <v>5.9341613601004681</v>
       </c>
       <c r="D6" s="1">
-        <v>4.9399535749999997</v>
+        <v>4.7147117677659738</v>
       </c>
       <c r="E6" s="1">
-        <v>4.7093637020000001</v>
+        <v>2.9582981575169054</v>
       </c>
       <c r="F6" s="1">
-        <v>4.0197831759999998</v>
+        <v>2.0812837364150862</v>
       </c>
       <c r="G6" s="1">
-        <v>2.4101597020000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+        <v>1.1986391469328441</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C7" s="1">
-        <v>5.4441473690000004</v>
+        <v>6.745167581667542</v>
       </c>
       <c r="D7" s="1">
-        <v>5.3786918620000002</v>
+        <v>5.0089487024708008</v>
       </c>
       <c r="E7" s="1">
-        <v>4.6881941380000001</v>
+        <v>2.9947637465553663</v>
       </c>
       <c r="F7" s="1">
-        <v>3.8619557320000002</v>
+        <v>2.0796138939738325</v>
       </c>
       <c r="G7" s="1">
-        <v>2.2128948560000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="1">
-        <v>5.4734904230000003</v>
-      </c>
-      <c r="D8" s="1">
-        <v>5.2345898699999998</v>
-      </c>
-      <c r="G8" s="1">
-        <v>2.7409796399999999</v>
-      </c>
-      <c r="H8" s="1">
-        <v>1.6798413919999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+        <v>1.8914522420411801</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F12" s="1"/>
     </row>
   </sheetData>
@@ -684,131 +629,89 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0A85062-6DA0-48EF-A3C8-1E0A08B47DCF}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
       </c>
       <c r="C2">
-        <f>AVERAGE(alldata!C2:C31)</f>
-        <v>6.3142400488571431</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+        <v>5.0896866084578987</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>0.1</v>
       </c>
       <c r="C3">
-        <f>AVERAGE(alldata!D2:D33)</f>
-        <v>5.9824422908333332</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+        <v>3.6827950363819215</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="C4">
-        <f>AVERAGE(alldata!E2:E32)</f>
-        <v>4.9926276986666673</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+        <v>2.0511596994682173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="C5">
-        <f>AVERAGE(alldata!F2:F36)</f>
-        <v>3.7299047474999996</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+        <v>1.4496427748119212</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="C6">
-        <f>AVERAGE(alldata!G2:G33)</f>
-        <v>2.2580731447142854</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+        <v>0.94943378395272704</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7">
-        <f>AVERAGE(alldata!H2:H16)</f>
-        <v>1.6798413919999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <f>AVERAGE(alldata!M2:M10)</f>
-        <v>1.1670344370000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9">
-        <f>AVERAGE(alldata!N2:N11)</f>
-        <v>1.168250097</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <f>AVERAGE(alldata!Q2:Q12)</f>
-        <v>0.198152722</v>
+        <v>0.32576927895594626</v>
       </c>
     </row>
   </sheetData>
@@ -818,61 +721,59 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A09306A-C128-4C46-A2A9-B870884FC8C6}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
       <c r="E1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C2">
-        <f>_xlfn.STDEV.S(alldata!C2:C21)</f>
-        <v>1.5412027393927117</v>
+        <v>1.4397425745760963</v>
       </c>
       <c r="D2">
         <f>COUNT(alldata!C2:C22)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2">
         <f>C2/SQRT(D2)</f>
-        <v>0.58251988119494358</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.58777244477873214</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>0.1</v>
       </c>
       <c r="C3">
-        <f>_xlfn.STDEV.S(alldata!D2:D22)</f>
-        <v>1.0254554417691895</v>
+        <v>1.3658647420040693</v>
       </c>
       <c r="D3">
         <f>COUNT(alldata!D2:D23)</f>
@@ -880,19 +781,18 @@
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E7" si="0">C3/SQRT(D3)</f>
-        <v>0.41864043104913706</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.55761194592802665</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="C4">
-        <f>_xlfn.STDEV.S(alldata!E2:E22)</f>
-        <v>1.1115744920950357</v>
+        <v>1.0235132377433305</v>
       </c>
       <c r="D4">
         <f>COUNT(alldata!E2:E23)</f>
@@ -900,19 +800,18 @@
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>0.45379838612103518</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.41784752957584809</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="C5">
-        <f>_xlfn.STDEV.S(alldata!F2:F22)</f>
-        <v>1.1763936233491212</v>
+        <v>0.84408525708246795</v>
       </c>
       <c r="D5">
         <f>COUNT(alldata!F2:F23)</f>
@@ -920,107 +819,45 @@
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>0.48026068564486835</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.34459636320966791</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="C6">
-        <f>_xlfn.STDEV.S(alldata!G2:G23)</f>
-        <v>0.7897497483380217</v>
+        <v>0.67246458883410565</v>
       </c>
       <c r="D6">
         <f>COUNT(alldata!G2:G23)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>0.2984973474397502</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.2745325187890082</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
-      <c r="C7" t="e">
-        <f>_xlfn.STDEV.S(alldata!H2:H16)</f>
-        <v>#DIV/0!</v>
+      <c r="C7">
+        <v>0.21381625305726057</v>
       </c>
       <c r="D7">
         <f>COUNT(alldata!H2:H16)</f>
-        <v>1</v>
-      </c>
-      <c r="E7" t="e">
+        <v>4</v>
+      </c>
+      <c r="E7">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" t="e">
-        <f>_xlfn.STDEV.S(alldata!M2:M11)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D8">
-        <f>COUNT(alldata!M2:M12)</f>
-        <v>1</v>
-      </c>
-      <c r="E8" t="e">
-        <f>C8/SQRT(D8)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" t="e">
-        <f>_xlfn.STDEV.S(alldata!N2:N15)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D9">
-        <f>COUNT(alldata!N2:N14)</f>
-        <v>1</v>
-      </c>
-      <c r="E9" t="e">
-        <f>C9/SQRT(D9)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" t="e">
-        <f>_xlfn.STDEV.S(alldata!Q2:Q13)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D10">
-        <f>COUNT(alldata!Q2:Q13)</f>
-        <v>1</v>
-      </c>
-      <c r="E10" t="e">
-        <f>C10/SQRT(D10)</f>
-        <v>#DIV/0!</v>
+        <v>0.10690812652863028</v>
       </c>
     </row>
   </sheetData>

</xml_diff>